<commit_message>
Updates in Viewing attachments
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1573">
   <si>
     <t>Trading</t>
   </si>
@@ -8637,6 +8637,51 @@
   </si>
   <si>
     <t>2019-04-16</t>
+  </si>
+  <si>
+    <t>2019-04-01</t>
+  </si>
+  <si>
+    <t>2019-04-09</t>
+  </si>
+  <si>
+    <t>2019-04-15</t>
+  </si>
+  <si>
+    <t>qq</t>
+  </si>
+  <si>
+    <t>2019-04-23</t>
+  </si>
+  <si>
+    <t>ghfgh</t>
+  </si>
+  <si>
+    <t>7fghj</t>
+  </si>
+  <si>
+    <t>786ghj</t>
+  </si>
+  <si>
+    <t>2019-04-03</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>hjhjk</t>
+  </si>
+  <si>
+    <t>Unit3</t>
+  </si>
+  <si>
+    <t>2019-04-17</t>
+  </si>
+  <si>
+    <t>2019-04-10</t>
+  </si>
+  <si>
+    <t>2019-04-18</t>
   </si>
 </sst>
 </file>
@@ -9034,7 +9079,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N1243"/>
+  <dimension ref="A1:N1272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -59256,6 +59301,1282 @@
       </c>
       <c r="N1243" s="4">
         <v>12</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:14">
+      <c r="A1244" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1244" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1244" s="4">
+        <v>1212</v>
+      </c>
+      <c r="D1244" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1244" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1244" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1244" s="4">
+        <v>34</v>
+      </c>
+      <c r="H1244" s="4">
+        <v>34</v>
+      </c>
+      <c r="I1244" s="4">
+        <v>34</v>
+      </c>
+      <c r="J1244" s="4">
+        <v>34</v>
+      </c>
+      <c r="K1244" s="4">
+        <v>34</v>
+      </c>
+      <c r="L1244" s="4">
+        <v>34</v>
+      </c>
+      <c r="M1244" s="4">
+        <v>34</v>
+      </c>
+      <c r="N1244" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:14">
+      <c r="A1245" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1245" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1245" s="4">
+        <v>1122222</v>
+      </c>
+      <c r="D1245" s="4">
+        <v>145</v>
+      </c>
+      <c r="E1245" s="4">
+        <v>125</v>
+      </c>
+      <c r="F1245" s="4">
+        <v>125</v>
+      </c>
+      <c r="G1245" s="4">
+        <v>126</v>
+      </c>
+      <c r="H1245" s="4">
+        <v>127</v>
+      </c>
+      <c r="I1245" s="4">
+        <v>1281</v>
+      </c>
+      <c r="J1245" s="4">
+        <v>129</v>
+      </c>
+      <c r="K1245" s="4">
+        <v>130</v>
+      </c>
+      <c r="L1245" s="4">
+        <v>140</v>
+      </c>
+      <c r="M1245" s="4">
+        <v>150</v>
+      </c>
+      <c r="N1245" s="4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:14">
+      <c r="A1246" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1246" s="4" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1246" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1246" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:14">
+      <c r="A1247" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1247" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1247" s="4">
+        <v>122</v>
+      </c>
+      <c r="D1247" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1247" s="4">
+        <v>112</v>
+      </c>
+      <c r="F1247" s="4">
+        <v>1212</v>
+      </c>
+      <c r="G1247" s="4">
+        <v>212</v>
+      </c>
+      <c r="H1247" s="4">
+        <v>1212</v>
+      </c>
+      <c r="I1247" s="4">
+        <v>1212</v>
+      </c>
+      <c r="J1247" s="4">
+        <v>1212</v>
+      </c>
+      <c r="K1247" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1247" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1247" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1247" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:14">
+      <c r="A1248" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1248" s="4" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1248" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1248" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:14">
+      <c r="A1249" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1249" s="4" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1249" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1249" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:14">
+      <c r="A1250" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1250" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1250" s="4">
+        <v>121</v>
+      </c>
+      <c r="D1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1250" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1250" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:14">
+      <c r="A1251" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1251" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1251" s="4">
+        <v>112</v>
+      </c>
+      <c r="H1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1251" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1251" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:14">
+      <c r="A1252" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1252" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1252" s="4" t="s">
+        <v>1561</v>
+      </c>
+      <c r="E1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1252" s="4">
+        <v>112</v>
+      </c>
+      <c r="H1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1252" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1252" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:14">
+      <c r="A1253" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1253" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1253" s="4">
+        <v>1212</v>
+      </c>
+      <c r="D1253" s="4">
+        <v>12213</v>
+      </c>
+      <c r="E1253" s="4">
+        <v>12312</v>
+      </c>
+      <c r="F1253" s="4">
+        <v>3123</v>
+      </c>
+      <c r="G1253" s="4">
+        <v>213</v>
+      </c>
+      <c r="H1253" s="4">
+        <v>21312</v>
+      </c>
+      <c r="I1253" s="4">
+        <v>3123123</v>
+      </c>
+      <c r="J1253" s="4">
+        <v>213</v>
+      </c>
+      <c r="K1253" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1253" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1253" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1253" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:14">
+      <c r="A1254" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1254" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1254" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1254" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:14">
+      <c r="A1255" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1255" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1255" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1255" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:14">
+      <c r="A1256" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1256" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1256" s="4">
+        <v>1121</v>
+      </c>
+      <c r="D1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1256" s="4">
+        <v>112</v>
+      </c>
+      <c r="K1256" s="4">
+        <v>121</v>
+      </c>
+      <c r="L1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1256" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1256" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:14">
+      <c r="A1257" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1257" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1257" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1257" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:14">
+      <c r="A1258" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1258" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1258" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="G1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="H1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="I1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1258" s="4">
+        <v>213</v>
+      </c>
+      <c r="L1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1258" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1258" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:14">
+      <c r="A1259" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1259" s="4" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="D1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1259" s="4">
+        <v>1233</v>
+      </c>
+      <c r="G1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="H1259" s="4">
+        <v>213</v>
+      </c>
+      <c r="I1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1259" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1259" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:14">
+      <c r="A1260" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1260" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1260" s="4">
+        <v>12</v>
+      </c>
+      <c r="D1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="G1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="H1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="I1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1260" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1260" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:14">
+      <c r="A1261" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1261" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1261" s="4">
+        <v>213</v>
+      </c>
+      <c r="D1261" s="4">
+        <v>213</v>
+      </c>
+      <c r="E1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="G1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="H1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="I1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1261" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1261" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:14">
+      <c r="A1262" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1262" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1262" s="4">
+        <v>56</v>
+      </c>
+      <c r="D1262" s="4" t="s">
+        <v>1563</v>
+      </c>
+      <c r="E1262" s="4">
+        <v>5656</v>
+      </c>
+      <c r="F1262" s="4">
+        <v>56</v>
+      </c>
+      <c r="G1262" s="4">
+        <v>67</v>
+      </c>
+      <c r="H1262" s="4">
+        <v>67</v>
+      </c>
+      <c r="I1262" s="4">
+        <v>67</v>
+      </c>
+      <c r="J1262" s="4">
+        <v>56</v>
+      </c>
+      <c r="K1262" s="4">
+        <v>56</v>
+      </c>
+      <c r="L1262" s="4">
+        <v>56</v>
+      </c>
+      <c r="M1262" s="4">
+        <v>65</v>
+      </c>
+      <c r="N1262" s="4" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:14">
+      <c r="A1263" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1263" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1263" s="4">
+        <v>787</v>
+      </c>
+      <c r="D1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="E1263" s="4">
+        <v>787</v>
+      </c>
+      <c r="F1263" s="4">
+        <v>787</v>
+      </c>
+      <c r="G1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="H1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="I1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="J1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="K1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="L1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="M1263" s="4">
+        <v>78</v>
+      </c>
+      <c r="N1263" s="4" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:14">
+      <c r="A1264" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1264" s="4" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C1264" s="4">
+        <v>565</v>
+      </c>
+      <c r="D1264" s="4">
+        <v>67</v>
+      </c>
+      <c r="E1264" s="4">
+        <v>67</v>
+      </c>
+      <c r="F1264" s="4">
+        <v>6767</v>
+      </c>
+      <c r="G1264" s="4">
+        <v>6767</v>
+      </c>
+      <c r="H1264" s="4">
+        <v>67</v>
+      </c>
+      <c r="I1264" s="4">
+        <v>67</v>
+      </c>
+      <c r="J1264" s="4">
+        <v>67</v>
+      </c>
+      <c r="K1264" s="4">
+        <v>89</v>
+      </c>
+      <c r="L1264" s="4">
+        <v>899</v>
+      </c>
+      <c r="M1264" s="4">
+        <v>89</v>
+      </c>
+      <c r="N1264" s="4" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:14">
+      <c r="A1265" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1265" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1265" s="4">
+        <v>778</v>
+      </c>
+      <c r="D1265" s="4">
+        <v>787</v>
+      </c>
+      <c r="E1265" s="4">
+        <v>878</v>
+      </c>
+      <c r="F1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="G1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="H1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="I1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="J1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="K1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="L1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="M1265" s="4">
+        <v>78</v>
+      </c>
+      <c r="N1265" s="4" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:14">
+      <c r="A1266" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1266" s="4" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C1266" s="4">
+        <v>321</v>
+      </c>
+      <c r="D1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1266" s="4">
+        <v>12312</v>
+      </c>
+      <c r="F1266" s="4">
+        <v>3123</v>
+      </c>
+      <c r="G1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="H1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="I1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1266" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1266" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:14">
+      <c r="A1267" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1267" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1267" s="4">
+        <v>1221</v>
+      </c>
+      <c r="D1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1267" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1267" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:14">
+      <c r="A1268" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1268" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C1268" s="4">
+        <v>23123</v>
+      </c>
+      <c r="D1268" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1268" s="4">
+        <v>213</v>
+      </c>
+      <c r="F1268" s="4">
+        <v>123</v>
+      </c>
+      <c r="G1268" s="4">
+        <v>213</v>
+      </c>
+      <c r="H1268" s="4">
+        <v>123</v>
+      </c>
+      <c r="I1268" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1268" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1268" s="4">
+        <v>213</v>
+      </c>
+      <c r="L1268" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1268" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1268" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:14">
+      <c r="A1269" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B1269" s="4" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C1269" s="4">
+        <v>1212</v>
+      </c>
+      <c r="D1269" s="4">
+        <v>1212</v>
+      </c>
+      <c r="E1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="F1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="G1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="H1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="I1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="J1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="K1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="L1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1269" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1269" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:14">
+      <c r="A1270" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B1270" s="4" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C1270" s="4">
+        <v>123123</v>
+      </c>
+      <c r="D1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="G1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="H1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="I1270" s="4">
+        <v>213</v>
+      </c>
+      <c r="J1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1270" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1270" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:14">
+      <c r="A1271" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B1271" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C1271" s="4">
+        <v>21312321</v>
+      </c>
+      <c r="D1271" s="4">
+        <v>321312</v>
+      </c>
+      <c r="E1271" s="4">
+        <v>3123</v>
+      </c>
+      <c r="F1271" s="4">
+        <v>123123</v>
+      </c>
+      <c r="G1271" s="4">
+        <v>21312</v>
+      </c>
+      <c r="H1271" s="4">
+        <v>3123</v>
+      </c>
+      <c r="I1271" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1271" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1271" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1271" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1271" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1271" s="4">
+        <v>12312</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:14">
+      <c r="A1272" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B1272" s="4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C1272" s="4">
+        <v>123</v>
+      </c>
+      <c r="D1272" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1272" s="4">
+        <v>123123</v>
+      </c>
+      <c r="F1272" s="4">
+        <v>213</v>
+      </c>
+      <c r="G1272" s="4">
+        <v>12312</v>
+      </c>
+      <c r="H1272" s="4">
+        <v>3123</v>
+      </c>
+      <c r="I1272" s="4">
+        <v>123</v>
+      </c>
+      <c r="J1272" s="4">
+        <v>123</v>
+      </c>
+      <c r="K1272" s="4">
+        <v>123</v>
+      </c>
+      <c r="L1272" s="4">
+        <v>123</v>
+      </c>
+      <c r="M1272" s="4">
+        <v>123</v>
+      </c>
+      <c r="N1272" s="4">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated export and search Functions
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Trading</t>
   </si>
@@ -29,9 +29,6 @@
     <t>Interval</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Plant Available Capacity(MW)</t>
   </si>
   <si>
@@ -62,22 +59,82 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Unit3</t>
-  </si>
-  <si>
-    <t>2019-04-17</t>
-  </si>
-  <si>
-    <t>2019-04-09</t>
-  </si>
-  <si>
-    <t>2019-04-10</t>
-  </si>
-  <si>
-    <t>2019-04-18</t>
-  </si>
-  <si>
-    <t>2019-04-22</t>
+    <t>Unit1</t>
+  </si>
+  <si>
+    <t>2019-05-06</t>
+  </si>
+  <si>
+    <t>0:00</t>
+  </si>
+  <si>
+    <t>1:00</t>
+  </si>
+  <si>
+    <t>2:00</t>
+  </si>
+  <si>
+    <t>3:00</t>
+  </si>
+  <si>
+    <t>4:00</t>
+  </si>
+  <si>
+    <t>5:00</t>
+  </si>
+  <si>
+    <t>6:00</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>8:00</t>
+  </si>
+  <si>
+    <t>9:00</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>22:00</t>
+  </si>
+  <si>
+    <t>23:00</t>
   </si>
 </sst>
 </file>
@@ -475,7 +532,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -483,7 +540,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="2"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -499,9 +556,8 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -541,22 +597,19 @@
       <c r="M2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4">
-        <v>1212</v>
-      </c>
       <c r="D3" s="4">
-        <v>1212</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4">
         <v>12</v>
@@ -585,228 +638,948 @@
       <c r="M3" s="4">
         <v>12</v>
       </c>
-      <c r="N3" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4">
-        <v>123123</v>
-      </c>
       <c r="D4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="F4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="H4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="I4" s="4">
-        <v>213</v>
+        <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="K4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="L4" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="M4" s="4">
-        <v>123</v>
-      </c>
-      <c r="N4" s="4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4">
-        <v>21312321</v>
-      </c>
       <c r="D5" s="4">
-        <v>321312</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4">
-        <v>3123</v>
+        <v>12</v>
       </c>
       <c r="F5" s="4">
-        <v>123123</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4">
-        <v>21312</v>
+        <v>12</v>
       </c>
       <c r="H5" s="4">
-        <v>3123</v>
+        <v>12</v>
       </c>
       <c r="I5" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="J5" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="K5" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="L5" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="M5" s="4">
-        <v>123</v>
-      </c>
-      <c r="N5" s="4">
-        <v>12312</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4">
-        <v>123</v>
-      </c>
       <c r="D6" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4">
-        <v>123123</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4">
-        <v>213</v>
+        <v>12</v>
       </c>
       <c r="G6" s="4">
-        <v>12312</v>
+        <v>12</v>
       </c>
       <c r="H6" s="4">
-        <v>3123</v>
+        <v>12</v>
       </c>
       <c r="I6" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="J6" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="K6" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="L6" s="4">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="M6" s="4">
-        <v>123</v>
-      </c>
-      <c r="N6" s="4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4">
-        <v>111</v>
-      </c>
       <c r="D7" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G7" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" s="4">
         <v>12</v>
       </c>
       <c r="I7" s="4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J7" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K7" s="4">
         <v>12</v>
       </c>
       <c r="L7" s="4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="M7" s="4">
-        <v>1</v>
-      </c>
-      <c r="N7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4">
-        <v>444</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="D8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L8" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="M8" s="4">
-        <v>4</v>
-      </c>
-      <c r="N8" s="4">
-        <v>4</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4">
+        <v>12</v>
+      </c>
+      <c r="I9" s="4">
+        <v>12</v>
+      </c>
+      <c r="J9" s="4">
+        <v>12</v>
+      </c>
+      <c r="K9" s="4">
+        <v>12</v>
+      </c>
+      <c r="L9" s="4">
+        <v>12</v>
+      </c>
+      <c r="M9" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4">
+        <v>12</v>
+      </c>
+      <c r="F10" s="4">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4">
+        <v>12</v>
+      </c>
+      <c r="H10" s="4">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4">
+        <v>12</v>
+      </c>
+      <c r="J10" s="4">
+        <v>12</v>
+      </c>
+      <c r="K10" s="4">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4">
+        <v>12</v>
+      </c>
+      <c r="M10" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4">
+        <v>12</v>
+      </c>
+      <c r="G11" s="4">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4">
+        <v>12</v>
+      </c>
+      <c r="I11" s="4">
+        <v>12</v>
+      </c>
+      <c r="J11" s="4">
+        <v>12</v>
+      </c>
+      <c r="K11" s="4">
+        <v>12</v>
+      </c>
+      <c r="L11" s="4">
+        <v>12</v>
+      </c>
+      <c r="M11" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4">
+        <v>12</v>
+      </c>
+      <c r="H12" s="4">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4">
+        <v>12</v>
+      </c>
+      <c r="J12" s="4">
+        <v>12</v>
+      </c>
+      <c r="K12" s="4">
+        <v>12</v>
+      </c>
+      <c r="L12" s="4">
+        <v>12</v>
+      </c>
+      <c r="M12" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4">
+        <v>12</v>
+      </c>
+      <c r="F13" s="4">
+        <v>12</v>
+      </c>
+      <c r="G13" s="4">
+        <v>12</v>
+      </c>
+      <c r="H13" s="4">
+        <v>12</v>
+      </c>
+      <c r="I13" s="4">
+        <v>12</v>
+      </c>
+      <c r="J13" s="4">
+        <v>12</v>
+      </c>
+      <c r="K13" s="4">
+        <v>12</v>
+      </c>
+      <c r="L13" s="4">
+        <v>12</v>
+      </c>
+      <c r="M13" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4">
+        <v>12</v>
+      </c>
+      <c r="G14" s="4">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4">
+        <v>12</v>
+      </c>
+      <c r="I14" s="4">
+        <v>12</v>
+      </c>
+      <c r="J14" s="4">
+        <v>12</v>
+      </c>
+      <c r="K14" s="4">
+        <v>12</v>
+      </c>
+      <c r="L14" s="4">
+        <v>12</v>
+      </c>
+      <c r="M14" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4">
+        <v>12</v>
+      </c>
+      <c r="F15" s="4">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4">
+        <v>12</v>
+      </c>
+      <c r="H15" s="4">
+        <v>12</v>
+      </c>
+      <c r="I15" s="4">
+        <v>12</v>
+      </c>
+      <c r="J15" s="4">
+        <v>12</v>
+      </c>
+      <c r="K15" s="4">
+        <v>12</v>
+      </c>
+      <c r="L15" s="4">
+        <v>12</v>
+      </c>
+      <c r="M15" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12</v>
+      </c>
+      <c r="E16" s="4">
+        <v>12</v>
+      </c>
+      <c r="F16" s="4">
+        <v>12</v>
+      </c>
+      <c r="G16" s="4">
+        <v>12</v>
+      </c>
+      <c r="H16" s="4">
+        <v>12</v>
+      </c>
+      <c r="I16" s="4">
+        <v>12</v>
+      </c>
+      <c r="J16" s="4">
+        <v>12</v>
+      </c>
+      <c r="K16" s="4">
+        <v>12</v>
+      </c>
+      <c r="L16" s="4">
+        <v>12</v>
+      </c>
+      <c r="M16" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="4">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4">
+        <v>12</v>
+      </c>
+      <c r="F17" s="4">
+        <v>12</v>
+      </c>
+      <c r="G17" s="4">
+        <v>12</v>
+      </c>
+      <c r="H17" s="4">
+        <v>12</v>
+      </c>
+      <c r="I17" s="4">
+        <v>12</v>
+      </c>
+      <c r="J17" s="4">
+        <v>12</v>
+      </c>
+      <c r="K17" s="4">
+        <v>12</v>
+      </c>
+      <c r="L17" s="4">
+        <v>12</v>
+      </c>
+      <c r="M17" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="4">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4">
+        <v>12</v>
+      </c>
+      <c r="F18" s="4">
+        <v>12</v>
+      </c>
+      <c r="G18" s="4">
+        <v>12</v>
+      </c>
+      <c r="H18" s="4">
+        <v>12</v>
+      </c>
+      <c r="I18" s="4">
+        <v>12</v>
+      </c>
+      <c r="J18" s="4">
+        <v>12</v>
+      </c>
+      <c r="K18" s="4">
+        <v>12</v>
+      </c>
+      <c r="L18" s="4">
+        <v>12</v>
+      </c>
+      <c r="M18" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4">
+        <v>12</v>
+      </c>
+      <c r="F19" s="4">
+        <v>12</v>
+      </c>
+      <c r="G19" s="4">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4">
+        <v>12</v>
+      </c>
+      <c r="I19" s="4">
+        <v>12</v>
+      </c>
+      <c r="J19" s="4">
+        <v>12</v>
+      </c>
+      <c r="K19" s="4">
+        <v>12</v>
+      </c>
+      <c r="L19" s="4">
+        <v>12</v>
+      </c>
+      <c r="M19" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="4">
+        <v>12</v>
+      </c>
+      <c r="E20" s="4">
+        <v>12</v>
+      </c>
+      <c r="F20" s="4">
+        <v>12</v>
+      </c>
+      <c r="G20" s="4">
+        <v>12</v>
+      </c>
+      <c r="H20" s="4">
+        <v>12</v>
+      </c>
+      <c r="I20" s="4">
+        <v>12</v>
+      </c>
+      <c r="J20" s="4">
+        <v>12</v>
+      </c>
+      <c r="K20" s="4">
+        <v>12</v>
+      </c>
+      <c r="L20" s="4">
+        <v>12</v>
+      </c>
+      <c r="M20" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4">
+        <v>12</v>
+      </c>
+      <c r="F21" s="4">
+        <v>12</v>
+      </c>
+      <c r="G21" s="4">
+        <v>12</v>
+      </c>
+      <c r="H21" s="4">
+        <v>12</v>
+      </c>
+      <c r="I21" s="4">
+        <v>12</v>
+      </c>
+      <c r="J21" s="4">
+        <v>12</v>
+      </c>
+      <c r="K21" s="4">
+        <v>12</v>
+      </c>
+      <c r="L21" s="4">
+        <v>12</v>
+      </c>
+      <c r="M21" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="4">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4">
+        <v>12</v>
+      </c>
+      <c r="F22" s="4">
+        <v>12</v>
+      </c>
+      <c r="G22" s="4">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4">
+        <v>12</v>
+      </c>
+      <c r="I22" s="4">
+        <v>12</v>
+      </c>
+      <c r="J22" s="4">
+        <v>12</v>
+      </c>
+      <c r="K22" s="4">
+        <v>12</v>
+      </c>
+      <c r="L22" s="4">
+        <v>12</v>
+      </c>
+      <c r="M22" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="4">
+        <v>12</v>
+      </c>
+      <c r="E23" s="4">
+        <v>12</v>
+      </c>
+      <c r="F23" s="4">
+        <v>12</v>
+      </c>
+      <c r="G23" s="4">
+        <v>12</v>
+      </c>
+      <c r="H23" s="4">
+        <v>12</v>
+      </c>
+      <c r="I23" s="4">
+        <v>12</v>
+      </c>
+      <c r="J23" s="4">
+        <v>12</v>
+      </c>
+      <c r="K23" s="4">
+        <v>12</v>
+      </c>
+      <c r="L23" s="4">
+        <v>12</v>
+      </c>
+      <c r="M23" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="4">
+        <v>12</v>
+      </c>
+      <c r="E24" s="4">
+        <v>12</v>
+      </c>
+      <c r="F24" s="4">
+        <v>12</v>
+      </c>
+      <c r="G24" s="4">
+        <v>12</v>
+      </c>
+      <c r="H24" s="4">
+        <v>12</v>
+      </c>
+      <c r="I24" s="4">
+        <v>12</v>
+      </c>
+      <c r="J24" s="4">
+        <v>12</v>
+      </c>
+      <c r="K24" s="4">
+        <v>12</v>
+      </c>
+      <c r="L24" s="4">
+        <v>12</v>
+      </c>
+      <c r="M24" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4">
+        <v>12</v>
+      </c>
+      <c r="E25" s="4">
+        <v>12</v>
+      </c>
+      <c r="F25" s="4">
+        <v>12</v>
+      </c>
+      <c r="G25" s="4">
+        <v>12</v>
+      </c>
+      <c r="H25" s="4">
+        <v>12</v>
+      </c>
+      <c r="I25" s="4">
+        <v>12</v>
+      </c>
+      <c r="J25" s="4">
+        <v>12</v>
+      </c>
+      <c r="K25" s="4">
+        <v>12</v>
+      </c>
+      <c r="L25" s="4">
+        <v>12</v>
+      </c>
+      <c r="M25" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4">
+        <v>12</v>
+      </c>
+      <c r="E26" s="4">
+        <v>12</v>
+      </c>
+      <c r="F26" s="4">
+        <v>12</v>
+      </c>
+      <c r="G26" s="4">
+        <v>12</v>
+      </c>
+      <c r="H26" s="4">
+        <v>12</v>
+      </c>
+      <c r="I26" s="4">
+        <v>12</v>
+      </c>
+      <c r="J26" s="4">
+        <v>12</v>
+      </c>
+      <c r="K26" s="4">
+        <v>12</v>
+      </c>
+      <c r="L26" s="4">
+        <v>12</v>
+      </c>
+      <c r="M26" s="4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>